<commit_message>
-Updated the AGE-WELL budget template
Former-commit-id: 7ca9eb1fc3565b0ce59f3023c229882fe7263999
</commit_message>
<xml_diff>
--- a/data/AGE-WELL Budget.xlsx
+++ b/data/AGE-WELL Budget.xlsx
@@ -9,18 +9,20 @@
   </bookViews>
   <sheets>
     <sheet name="Overall Project Budget" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="NI 1" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Overall Project Budget'!$A$1:$M$29</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Overall Project Budget'!$A$1:$M$29</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Overall Project Budget'!$A$1:$M$29</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Overall Project Budget'!$A$1:$M$29</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
   <si>
     <t>AGE-WELL NCE Proposal Budget Request</t>
   </si>
@@ -554,7 +556,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -628,7 +630,7 @@
   <dimension ref="1:26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -3137,4 +3139,449 @@
     <brk id="29" man="true" max="16383" min="0"/>
   </rowBreaks>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="27" t="n">
+        <f aca="false">B11*C11</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="28"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="30" t="n">
+        <f aca="false">SUM(E11:F11)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="31" t="n">
+        <f aca="false">SUM(D11,G11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="27" t="n">
+        <f aca="false">B12*C12</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="28"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="33" t="n">
+        <f aca="false">SUM(E12:F12)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="31" t="n">
+        <f aca="false">SUM(D12,G12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="32"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="27" t="n">
+        <f aca="false">B13*C13</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="28"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="30" t="n">
+        <f aca="false">SUM(E13:F13)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="31" t="n">
+        <f aca="false">SUM(D13,G13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="34"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="31" t="n">
+        <f aca="false">SUM(D14,G14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="27" t="n">
+        <f aca="false">B15*C15</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="38"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="30" t="n">
+        <f aca="false">SUM(E15:F15)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="31" t="n">
+        <f aca="false">SUM(D15,G15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="32"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27" t="n">
+        <f aca="false">B16*C16</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="30" t="n">
+        <f aca="false">SUM(E16:F16)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="31" t="n">
+        <f aca="false">SUM(D16,G16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="40"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27" t="n">
+        <f aca="false">B17*C17</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="30" t="n">
+        <f aca="false">SUM(E17:F17)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="31" t="n">
+        <f aca="false">SUM(D17,G17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="34"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27" t="n">
+        <f aca="false">C18</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="28"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="30" t="n">
+        <f aca="false">SUM(E18:F18)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="31" t="n">
+        <f aca="false">SUM(D18,G18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="34"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="27" t="n">
+        <f aca="false">C19</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="28"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="30" t="n">
+        <f aca="false">SUM(E19:F19)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="31" t="n">
+        <f aca="false">SUM(D19,G19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="34"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="27" t="n">
+        <f aca="false">C20</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="28"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="30" t="n">
+        <f aca="false">SUM(E20:F20)</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="31" t="n">
+        <f aca="false">SUM(D20,G20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="34"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="27" t="n">
+        <f aca="false">C21</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="28"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="30" t="n">
+        <f aca="false">SUM(E21:F21)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="31" t="n">
+        <f aca="false">SUM(D21,G21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43" t="n">
+        <f aca="false">SUM(C10:C21)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="44" t="n">
+        <f aca="false">SUM(D11:D21)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="27" t="n">
+        <f aca="false">SUM(E11:E21)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="27" t="n">
+        <f aca="false">SUM(F11:F21)</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="27" t="n">
+        <f aca="false">SUM(G11:G21)</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="31" t="n">
+        <f aca="false">SUM(D22,G22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="45"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A24:H24"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
-Updated the AGE-WELL Budget
Former-commit-id: 40d1e137e15f34366f6b77c0d2f9c2f676668420
</commit_message>
<xml_diff>
--- a/data/AGE-WELL Budget.xlsx
+++ b/data/AGE-WELL Budget.xlsx
@@ -16,6 +16,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Overall Project Budget'!$A$1:$M$29</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Overall Project Budget'!$A$1:$M$29</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Overall Project Budget'!$A$1:$M$29</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Overall Project Budget'!$A$1:$M$29</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -42,7 +43,7 @@
     <t>Names of Project Investigators Receiving Funding</t>
   </si>
   <si>
-    <t>April 1, 2016 - March 31, 2017</t>
+    <t>April 1, 2017 - March 31, 2018</t>
   </si>
   <si>
     <t>Expenditure Categories</t>
@@ -556,7 +557,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -630,7 +631,7 @@
   <dimension ref="1:26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -3149,7 +3150,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>